<commit_message>
addedd 2weekly and 4weekly cat A packages
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="24" windowWidth="14340" windowHeight="4512" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="4512" windowWidth="14340" xWindow="384" yWindow="24"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="57">
   <si>
     <t>TC</t>
   </si>
@@ -194,6 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,48 +242,48 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -296,10 +297,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -457,7 +458,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -466,13 +467,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -482,7 +483,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -491,7 +492,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -500,7 +501,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -510,12 +511,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -546,7 +547,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -565,7 +566,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -577,7 +578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -586,10 +587,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -606,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -620,7 +621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="3" s="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -634,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="4" s="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -648,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row ht="43.2" r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -662,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="6" s="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -676,7 +677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -690,7 +691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row ht="72" r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -714,13 +715,13 @@
       <c r="E13" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -729,12 +730,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.44140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="18.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -921,13 +922,13 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -936,19 +937,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="50.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="50.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -989,7 +990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="10" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>55</v>
       </c>
@@ -1027,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>55</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>55</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>55</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>55</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="8" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="9" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>55</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="10" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>55</v>
       </c>
@@ -1309,23 +1310,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId10" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1334,20 +1335,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="54.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="49.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="54.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>55</v>
       </c>
@@ -1431,8 +1432,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated payroll script and TLS continue button enhancement work
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515" activeTab="2"/>
+    <workbookView activeTab="2" windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="57">
   <si>
     <t>TC</t>
   </si>
@@ -199,6 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,48 +247,48 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -304,10 +305,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -342,7 +343,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,7 +395,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,7 +500,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -508,13 +509,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -524,7 +525,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -533,7 +534,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -542,7 +543,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -552,12 +553,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -588,7 +589,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -607,7 +608,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -619,7 +620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -628,10 +629,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,7 +649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -662,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -676,7 +677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -690,7 +691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -704,7 +705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -718,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -732,7 +733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -756,13 +757,13 @@
       <c r="E13" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -771,12 +772,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -963,13 +964,13 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
@@ -978,19 +979,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="50.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="50.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="10" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>54</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>54</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>54</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>54</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="8" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="9" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>54</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="10" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>54</v>
       </c>
@@ -1351,23 +1352,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId10" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1376,20 +1377,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="54.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="49.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="54.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
@@ -1473,8 +1474,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Input Files and XML files path changes checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
-    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
-    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
+    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
   <si>
     <t>TC</t>
   </si>
@@ -87,33 +87,6 @@
     <t>Two Weekly</t>
   </si>
   <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 101</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 102</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 103</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 104</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 105</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 106</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 107</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 108</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 109</t>
-  </si>
-  <si>
     <t>TestReports</t>
   </si>
   <si>
@@ -186,20 +159,46 @@
     <t>7</t>
   </si>
   <si>
-    <t>DO NOT TOUCH PAYROLL AUTOMATION EMPLOYER_17/18</t>
-  </si>
-  <si>
-    <t>TwoWeekly_Payroll</t>
-  </si>
-  <si>
     <t>F:\\Automation_TestResults\\Payroll_Tax_NI_Directors_TestReports 201718\\201718 Payroll National Insurance calculation Test result.xlsx</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 441</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 442</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 443</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 444</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 445</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 446</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 447</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 448</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 449</t>
+  </si>
+  <si>
+    <t>DONT TOUCH AUTO NI2WCA EMPLOYER</t>
+  </si>
+  <si>
+    <t>NI2WCA_Payroll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,48 +246,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -305,10 +300,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -343,7 +338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,7 +390,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +495,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -509,13 +504,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -525,7 +520,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -534,7 +529,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -543,7 +538,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -553,12 +548,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -589,7 +584,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -608,7 +603,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -620,7 +615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -629,10 +624,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,21 +644,21 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -677,12 +672,12 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -691,12 +686,12 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -705,7 +700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -719,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -733,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="75" r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -757,27 +752,27 @@
       <c r="E13" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="42.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,8 +799,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
+      <c r="A2" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -821,8 +816,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
+      <c r="A3" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
@@ -838,8 +833,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
+      <c r="A4" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
@@ -856,8 +851,8 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>24</v>
+      <c r="A5" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
@@ -874,8 +869,8 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>25</v>
+      <c r="A6" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
@@ -892,8 +887,8 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>26</v>
+      <c r="A7" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
@@ -910,8 +905,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
+      <c r="A8" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
@@ -928,8 +923,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>28</v>
+      <c r="A9" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
@@ -946,8 +941,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
+      <c r="A10" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
@@ -964,63 +959,63 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H10" activeCellId="1" sqref="H10 H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="50.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="50.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="50.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>2</v>
@@ -1032,397 +1027,399 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:13" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="8" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="9" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="10" s="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="D10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>49</v>
+      <c r="E10" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId10" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="A3:A10" r:id="rId11" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId10" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="54.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="5" width="22.28515625" collapsed="true"/>
+    <col min="1" max="1" width="49.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="54.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.28515625" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>2</v>
@@ -1434,48 +1431,49 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="12" t="s">
+    <row r="2" spans="1:14" s="9" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>49</v>
+      <c r="E2" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pagination code for input script for Payroll NI Module is implemented
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
+    <workbookView xWindow="396" yWindow="36" windowWidth="14340" windowHeight="4512" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
-    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
-    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
+    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
   <si>
     <t>TC</t>
   </si>
@@ -198,8 +193,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,48 +241,48 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -305,10 +299,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -343,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,26 +370,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -428,23 +405,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,7 +460,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -509,13 +469,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -525,7 +485,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -534,7 +494,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -543,7 +503,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -553,12 +513,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -589,7 +549,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -608,7 +568,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -620,22 +580,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="48.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -663,7 +623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -677,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -691,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -705,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -719,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -733,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row ht="75" r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -747,40 +707,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E13" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.44140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -803,8 +763,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -820,8 +780,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -837,8 +797,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -855,8 +815,8 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -873,8 +833,8 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -891,8 +851,8 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -909,8 +869,8 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -927,8 +887,8 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -945,8 +905,8 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -963,35 +923,38 @@
       </c>
       <c r="H10" s="2"/>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H10" activeCellId="1" sqref="H10 H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="50.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="50.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="50.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="50.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -1032,7 +995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
@@ -1070,7 +1033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>54</v>
       </c>
@@ -1105,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>54</v>
       </c>
@@ -1140,7 +1103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -1175,7 +1138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>54</v>
       </c>
@@ -1210,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>54</v>
       </c>
@@ -1245,7 +1208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="8" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
@@ -1280,7 +1243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="9" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>54</v>
       </c>
@@ -1315,7 +1278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="10" s="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>54</v>
       </c>
@@ -1352,45 +1315,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId10" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="54.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="5" width="22.28515625" collapsed="true"/>
+    <col min="1" max="1" width="49.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="54.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.33203125" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -1434,7 +1397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
@@ -1474,8 +1437,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented best logic for Payroll NI Module for input script pagination
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515" activeTab="3"/>
+    <workbookView activeTab="1" windowHeight="4512" windowWidth="14340" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NI2WeeklyCat_A" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NI2WeeklyCat_A" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="57">
   <si>
     <t>TC</t>
   </si>
@@ -198,7 +193,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,44 +242,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -300,10 +296,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -338,7 +334,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,26 +367,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,23 +402,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,7 +457,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -504,13 +466,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -520,7 +482,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -529,7 +491,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -538,7 +500,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -548,12 +510,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -584,7 +546,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -603,7 +565,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -615,22 +577,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -658,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="15" r="3" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -672,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="15" r="4" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -686,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -700,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="15" r="6" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -714,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -728,7 +690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -742,37 +704,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E13" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="18.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -959,34 +921,34 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="50.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="50.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1027,7 +989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -1065,7 +1027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>55</v>
       </c>
@@ -1100,7 +1062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>55</v>
       </c>
@@ -1135,7 +1097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>55</v>
       </c>
@@ -1170,7 +1132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>55</v>
       </c>
@@ -1205,7 +1167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>55</v>
       </c>
@@ -1240,7 +1202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="8" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>55</v>
       </c>
@@ -1275,7 +1237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="9" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>55</v>
       </c>
@@ -1310,7 +1272,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="10" s="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>55</v>
       </c>
@@ -1347,47 +1309,47 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId10" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="A3:A10" r:id="rId11" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId10" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId11" ref="A3:A10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId12" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="54.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="49.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="54.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1431,7 +1393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -1471,9 +1433,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automation Reg Org Pagination issue fix
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 2WeeklyCatA201718.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="4512" windowWidth="14340" xWindow="396" yWindow="36"/>
+    <workbookView activeTab="1" windowHeight="4512" windowWidth="14340" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -12,12 +12,12 @@
     <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
     <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="57">
   <si>
     <t>TC</t>
   </si>
@@ -157,9 +157,6 @@
     <t>F:\\Automation_TestResults\\Payroll_Tax_NI_Directors_TestReports 201718\\201718 Payroll National Insurance calculation Test result.xlsx</t>
   </si>
   <si>
-    <t>NI2WCB_Payroll</t>
-  </si>
-  <si>
     <t>DO NOT TOUCH AUTOMATION EMP 441</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>DONT TOUCH AUTO NI2WCA EMPLOYER</t>
+  </si>
+  <si>
+    <t>NI2WCA_Payroll</t>
   </si>
 </sst>
 </file>
@@ -270,8 +270,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
@@ -723,13 +723,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="42.109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="14.6640625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="5" width="18.44140625" collapsed="true"/>
@@ -737,7 +737,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="7.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -760,9 +760,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>47</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -777,9 +777,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>48</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
@@ -794,9 +794,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>49</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
@@ -812,9 +812,9 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>50</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
@@ -830,9 +830,9 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>51</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
@@ -848,9 +848,9 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>52</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
@@ -866,9 +866,9 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>53</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
@@ -884,9 +884,9 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>54</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
@@ -902,9 +902,9 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>55</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,15 +989,15 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>20</v>
@@ -1027,15 +1027,15 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="27.6" r="3" s="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>20</v>
@@ -1062,15 +1062,15 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="27.6" r="4" s="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>20</v>
@@ -1097,15 +1097,15 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="27.6" r="5" s="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>20</v>
@@ -1132,15 +1132,15 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="27.6" r="6" s="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>20</v>
@@ -1167,15 +1167,15 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="27.6" r="7" s="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>20</v>
@@ -1203,14 +1203,14 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="27.6" r="8" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>20</v>
@@ -1238,14 +1238,14 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="27.6" r="9" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>20</v>
@@ -1273,14 +1273,14 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="27.6" r="10" s="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>20</v>
@@ -1318,10 +1318,11 @@
     <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
     <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
     <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId10" ref="A2:A10"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId10" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId11" ref="A3:A10"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId11" verticalDpi="0"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId12" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1329,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,15 +1393,15 @@
         <v>11</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row customFormat="1" customHeight="1" ht="54.75" r="2" s="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>20</v>

</xml_diff>